<commit_message>
Initial commit with basic website structure.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koral/projects/excel-data-display/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9640519B-6F02-5B47-81C4-881CF97B481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{80672E1D-A976-6D43-88B9-E92341A0CDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="6" uniqueCount="6">
-  <si>
-    <t>Name,"Age","Occupation","Country"</t>
-  </si>
-  <si>
-    <t>John Doe,"28","Software Developer","USA"</t>
-  </si>
-  <si>
-    <t>Jane Smith,"34","Architect","Canada"</t>
-  </si>
-  <si>
-    <t>Robert Brown,"22","Student","UK"</t>
-  </si>
-  <si>
-    <t>Maria Garcia,"45","Teacher","Spain"</t>
-  </si>
-  <si>
-    <t>Xiu Ying,"30","Engineer","China"</t>
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="19" uniqueCount="19">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Architect</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Robert Brown</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Maria Garcia</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Xiu Ying</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>China</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -526,8 +565,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -882,41 +922,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>